<commit_message>
Optimized the AnnualSalary Method which in general is used by all Payroll modules to update annual salary And also modified Director as employee input script.
</commit_message>
<xml_diff>
--- a/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Suite IncomeTax_TCWeek1_204045VariablePay&Weekly50RL201718.xlsx
+++ b/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Suite IncomeTax_TCWeek1_204045VariablePay&Weekly50RL201718.xlsx
@@ -4,20 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="396" yWindow="276" windowWidth="14340" windowHeight="4272" activeTab="3"/>
+    <workbookView activeTab="3" windowHeight="4272" windowWidth="14340" xWindow="396" yWindow="276"/>
   </bookViews>
   <sheets>
-    <sheet name="first" sheetId="1" r:id="rId1"/>
-    <sheet name="GeneralTaxRateWeekly" sheetId="2" r:id="rId2"/>
-    <sheet name="ProcessPayrollForWeeklyTax" sheetId="4" r:id="rId3"/>
-    <sheet name="TestReports" sheetId="5" r:id="rId4"/>
+    <sheet name="first" r:id="rId1" sheetId="1"/>
+    <sheet name="GeneralTaxRateWeekly" r:id="rId2" sheetId="2"/>
+    <sheet name="ProcessPayrollForWeeklyTax" r:id="rId3" sheetId="4"/>
+    <sheet name="TestReports" r:id="rId4" sheetId="5"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="52">
   <si>
     <t>TC</t>
   </si>
@@ -179,6 +179,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -296,92 +297,92 @@
     </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="27">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" applyProtection="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyProtection="1" borderId="1" fillId="4" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyProtection="1" borderId="2" fillId="4" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyProtection="1" borderId="1" fillId="5" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyProtection="1" borderId="2" fillId="5" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyProtection="1" borderId="1" fillId="6" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyProtection="1" borderId="2" fillId="6" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyProtection="1" borderId="3" fillId="3" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyProtection="1" borderId="2" fillId="3" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyProtection="1" borderId="3" fillId="7" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyProtection="1" borderId="2" fillId="7" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="justify"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="justify" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="justify" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="2"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -398,10 +399,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -559,7 +560,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -568,13 +569,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -584,7 +585,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -593,7 +594,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -602,7 +603,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -612,12 +613,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -648,7 +649,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -667,7 +668,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -679,7 +680,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -688,13 +689,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="38.33203125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="33.5546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="31.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="38.33203125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="33.5546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.44140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -708,7 +709,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -722,7 +723,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -736,7 +737,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -750,7 +751,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -765,13 +766,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -780,14 +781,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="37.5546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20.109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="37.5546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="12.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="20.109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.6640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -813,7 +814,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="21.6" r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="26" t="s">
         <v>45</v>
       </c>
@@ -925,19 +926,19 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="C6" type="list">
       <formula1>$B$19:$B$20</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="C5" type="list">
       <formula1>$B$15:$B$16</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -946,17 +947,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="38.21875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="36.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.6640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.109375" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="40.44140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="25.5546875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="45.88671875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="38.21875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="36.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="14.6640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.109375" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="40.44140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="25.5546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="45.88671875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="18" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="15" r="1" s="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>28</v>
       </c>
@@ -997,7 +998,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="21" customFormat="1" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="43.2" r="2" s="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="26" t="s">
         <v>50</v>
       </c>
@@ -1032,7 +1033,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row ht="43.2" r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
         <v>50</v>
       </c>
@@ -1067,7 +1068,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row ht="43.2" r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="26" t="s">
         <v>50</v>
       </c>
@@ -1102,7 +1103,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row ht="43.2" r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="26" t="s">
         <v>50</v>
       </c>
@@ -1137,7 +1138,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row ht="43.2" r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="26" t="s">
         <v>50</v>
       </c>
@@ -1174,14 +1175,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2:A6" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2:A6"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -1190,15 +1191,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.21875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="35.44140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.88671875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="34" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="29.109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="46" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="35.21875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="35.44140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="14.88671875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="34.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="29.109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="46.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
@@ -1239,7 +1240,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="25" customFormat="1" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="43.2" r="2" s="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="26" t="s">
         <v>50</v>
       </c>
@@ -1276,8 +1277,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>